<commit_message>
#262 settings service (#13)
* Заменил загрузку хранилищ данных с адаптера работы с json на хранение в виде конфигурации.

* Исправил ошибку, возникающую при открытии основного окна с выбором репозиторияиз списка доступных.

* Добавил проверку на null в фабрики VM.

* Доработал подключение настроечных файлов.

* Доработал работу с App.xaml.cs

* Оптимизировал работу с хранилищами.

* fix

* Перевел логирование на Serilog.
Добавил вывод этапов запуска в консоль.

* Доработал получение списков хранилищ и заголовков репозитория через IOptions DI-контейнера.
Синхронизировал с работой репозитория для записи изменений в файл.

* Добавил комментарий.

* fix

* Доработал интерфейс настроек.
Добавил в интерфейсе настройку списка настроечных файлов. А также функционал открытия настроечных файлов и их переноса в другую директорию.
</commit_message>
<xml_diff>
--- a/Philadelphus.Presentation.Wpf.UI/Icons/Авторы.xlsx
+++ b/Philadelphus.Presentation.Wpf.UI/Icons/Авторы.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MelSV_Projects\Philadelphus\Philadelphus.WpfApplication\Philadelphus.WpfApplication\Philadelphus.WpfApplication\Icons\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MelSV_Projects\Philadelphus.General\Philadelphus.Presentation.Wpf.UI\Icons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FC7E769-39DA-4487-87A0-6871959C9BBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98800EDF-5CDD-49D9-969B-8B0CBE8205FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1035" yWindow="2175" windowWidth="16410" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="46">
   <si>
     <t>Сайт</t>
   </si>
@@ -154,6 +154,18 @@
   </si>
   <si>
     <t>https://icons8.ru/icon/H5fos0lujvMY/квадратный-корень-2</t>
+  </si>
+  <si>
+    <t>https://www.flaticon.com/free-icon/repair-tool_2760290?term=settings&amp;page=4&amp;position=48&amp;origin=search&amp;related_id=2760290</t>
+  </si>
+  <si>
+    <t>repair-tool.png</t>
+  </si>
+  <si>
+    <t>&lt;a href="https://www.flaticon.com/free-icons/repair" title="repair icons"&gt;Repair icons created by Ayub Irawan - Flaticon&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>settings_64.png</t>
   </si>
 </sst>
 </file>
@@ -219,10 +231,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -503,19 +516,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:E10"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34" customWidth="1"/>
-    <col min="5" max="5" width="31" customWidth="1"/>
+    <col min="1" max="1" width="26.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34" style="1" customWidth="1"/>
+    <col min="5" max="5" width="31" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -686,6 +699,23 @@
       </c>
       <c r="E10" s="1" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>